<commit_message>
Color coding and scale for combo analysis
</commit_message>
<xml_diff>
--- a/shareddata/MultiChoiceCombo.xlsx
+++ b/shareddata/MultiChoiceCombo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fhw108/Documents/gitrepos/ctsa-sustainability/shareddata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9AAB1C16-BD26-2E4D-B57E-5EBCF9F29864}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDE8D17-F125-624F-920D-82F7FAE3396F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12400" yWindow="29260" windowWidth="28800" windowHeight="17540" firstSheet="5" activeTab="15" xr2:uid="{7B827D7C-163A-B34E-B6BC-F543988253A9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{7B827D7C-163A-B34E-B6BC-F543988253A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Regulatory Compliance" sheetId="2" r:id="rId1"/>
@@ -111,7 +111,768 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="76">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -423,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32ED72A-FCFE-C547-9C58-3771F6891AC5}">
   <dimension ref="B1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -982,6 +1743,34 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:E17 I2:L17">
+    <cfRule type="cellIs" dxfId="63" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -991,7 +1780,7 @@
   <dimension ref="B1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1552,6 +2341,34 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:E17 H2:K17">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1561,7 +2378,7 @@
   <dimension ref="B1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2119,6 +2936,34 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:E17 H2:K17">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2128,7 +2973,7 @@
   <dimension ref="B1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="H2" sqref="H2:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2566,6 +3411,34 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:E9 H2:K17">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2575,7 +3448,7 @@
   <dimension ref="B1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3016,6 +3889,42 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:E9">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F9">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:K17">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3025,7 +3934,7 @@
   <dimension ref="B1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3583,6 +4492,34 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:E17 H2:K17">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3592,7 +4529,7 @@
   <dimension ref="B1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4150,6 +5087,34 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:E17 H2:K17">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4158,8 +5123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78A2979-E731-2445-A837-D690C92DB727}">
   <dimension ref="B1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4717,6 +5682,34 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:E17 H2:K17">
+    <cfRule type="cellIs" dxfId="70" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4726,7 +5719,7 @@
   <dimension ref="B1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5164,6 +6157,34 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:E17 I2:L9">
+    <cfRule type="cellIs" dxfId="55" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M9">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -5173,7 +6194,7 @@
   <dimension ref="B1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H17"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5731,6 +6752,34 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="I2:L17 B2:E17">
+    <cfRule type="cellIs" dxfId="48" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -5740,7 +6789,7 @@
   <dimension ref="B1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6298,6 +7347,34 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:E17 I2:L17">
+    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -6307,7 +7384,7 @@
   <dimension ref="B1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6869,6 +7946,34 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:E17 H2:K17">
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6878,7 +7983,7 @@
   <dimension ref="B1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7436,6 +8541,34 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:E17 H2:K17">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7445,7 +8578,7 @@
   <dimension ref="B1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8003,6 +9136,34 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:E17 H2:K17">
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8012,7 +9173,7 @@
   <dimension ref="B1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8570,6 +9731,34 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:E17 H2:K17">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8579,7 +9768,7 @@
   <dimension ref="B1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9140,6 +10329,34 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:E17 H2:K17">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>